<commit_message>
add deploy script from ignore
</commit_message>
<xml_diff>
--- a/LogLikePrior_Catalog/Catalog_Overview.xlsx
+++ b/LogLikePrior_Catalog/Catalog_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/CurveAware/LogLikePrior_Catalog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BCF29E-4444-B74D-9BA3-702F130E6FD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5C40CA-D940-BE4E-846A-239FC8E77BCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9380" yWindow="3840" windowWidth="28040" windowHeight="17440" xr2:uid="{2083A32E-6419-C843-8898-0AA7F7565E14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -113,6 +113,21 @@
   </si>
   <si>
     <t>r1 (ma1)</t>
+  </si>
+  <si>
+    <t>R_intermedMa_prior</t>
+  </si>
+  <si>
+    <t>R_intermedI0_prior</t>
+  </si>
+  <si>
+    <t>Log-Normal(0.69, 0.5)</t>
+  </si>
+  <si>
+    <t>Beta(10, 90)</t>
+  </si>
+  <si>
+    <t>Beta(50, 50)</t>
   </si>
 </sst>
 </file>
@@ -494,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C57432B-DA17-A647-A206-A6FC547ACFDA}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +593,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -595,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -603,12 +618,12 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -617,7 +632,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -633,6 +648,66 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update vignettes and pkg site
</commit_message>
<xml_diff>
--- a/LogLikePrior_Catalog/Catalog_Overview.xlsx
+++ b/LogLikePrior_Catalog/Catalog_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/CurveAware/LogLikePrior_Catalog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5C40CA-D940-BE4E-846A-239FC8E77BCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7D7289-0EA2-3443-9B2F-4C2DFE88FFB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9380" yWindow="3840" windowWidth="28040" windowHeight="17440" xr2:uid="{2083A32E-6419-C843-8898-0AA7F7565E14}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -58,18 +58,12 @@
     <t>Uniform(1, 10)</t>
   </si>
   <si>
-    <t>Log-Normal(0, 5)</t>
-  </si>
-  <si>
     <t>Uniform(0, 1)</t>
   </si>
   <si>
     <t>Cumulative</t>
   </si>
   <si>
-    <t>r1/ma2</t>
-  </si>
-  <si>
     <t>R_likelihood_cumulative</t>
   </si>
   <si>
@@ -103,54 +97,27 @@
     <t>Beta(500, 500)</t>
   </si>
   <si>
-    <t>True Value</t>
-  </si>
-  <si>
-    <t>0.2 (0.1)</t>
-  </si>
-  <si>
-    <t>Param Sims</t>
-  </si>
-  <si>
-    <t>r1 (ma1)</t>
-  </si>
-  <si>
-    <t>R_intermedMa_prior</t>
-  </si>
-  <si>
-    <t>R_intermedI0_prior</t>
-  </si>
-  <si>
-    <t>Log-Normal(0.69, 0.5)</t>
-  </si>
-  <si>
-    <t>Beta(10, 90)</t>
-  </si>
-  <si>
-    <t>Beta(50, 50)</t>
+    <t>ma1</t>
+  </si>
+  <si>
+    <t>R_reparameterize_Ma_prior</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>ma4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -160,7 +127,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,15 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,21 +470,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C57432B-DA17-A647-A206-A6FC547ACFDA}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,19 +497,13 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -556,47 +511,29 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -605,110 +542,96 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -739,29 +662,29 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>